<commit_message>
fix ICO in Linux
</commit_message>
<xml_diff>
--- a/data/Ленинский/ЗУ/data/points.xlsx
+++ b/data/Ленинский/ЗУ/data/points.xlsx
@@ -399,20 +399,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>54:35:061375:27</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D2" t="n">
-        <v>486368.23</v>
+        <v>486293.86</v>
       </c>
       <c r="E2" t="n">
-        <v>4194879.66</v>
+        <v>4194840.04</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3">
@@ -421,20 +421,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>54:35:061375:27</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D3" t="n">
-        <v>486332.43</v>
+        <v>486293.58</v>
       </c>
       <c r="E3" t="n">
-        <v>4194915.07</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.1</v>
+        <v>4194840.47</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -443,20 +445,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>54:35:061375:27</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="D4" t="n">
-        <v>486330.69</v>
+        <v>486294.71</v>
       </c>
       <c r="E4" t="n">
-        <v>4194913.66</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.1</v>
+        <v>4194840.58</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -465,20 +469,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>54:35:061375:27</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D5" t="n">
-        <v>486326.17</v>
+        <v>486293.86</v>
       </c>
       <c r="E5" t="n">
-        <v>4194910.03</v>
+        <v>4194840.04</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6">
@@ -487,20 +491,20 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>54:35:061375:27</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>486325.41</v>
+        <v>486280.32</v>
       </c>
       <c r="E6" t="n">
-        <v>4194909.41</v>
+        <v>4194861.75</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="7">
@@ -509,20 +513,20 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>54:35:061375:27</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>486323.33</v>
+        <v>486287.28</v>
       </c>
       <c r="E7" t="n">
-        <v>4194908.18</v>
+        <v>4194866.48</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="8">
@@ -531,20 +535,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>54:35:061375:27</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>486323.34</v>
+        <v>486299.2</v>
       </c>
       <c r="E8" t="n">
-        <v>4194907.14</v>
+        <v>4194875.36</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="9">
@@ -553,20 +557,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>54:35:061375:27</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D9" t="n">
-        <v>486323.54</v>
+        <v>486323.27</v>
       </c>
       <c r="E9" t="n">
-        <v>4194905.83</v>
+        <v>4194893.02</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="10">
@@ -575,20 +579,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>54:35:061375:27</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D10" t="n">
-        <v>486329.74</v>
+        <v>486323.56</v>
       </c>
       <c r="E10" t="n">
-        <v>4194897.48</v>
+        <v>4194893.22</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="11">
@@ -597,20 +601,20 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>54:35:061375:27</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D11" t="n">
-        <v>486323.56</v>
+        <v>486329.57</v>
       </c>
       <c r="E11" t="n">
-        <v>4194893.22</v>
+        <v>4194885.14</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="12">
@@ -619,20 +623,20 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>54:35:061375:27</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
-        <v>486329.57</v>
+        <v>486335.31</v>
       </c>
       <c r="E12" t="n">
-        <v>4194885.14</v>
+        <v>4194877.7</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="13">
@@ -641,20 +645,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>54:35:061375:27</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D13" t="n">
-        <v>486335.31</v>
+        <v>486345.35</v>
       </c>
       <c r="E13" t="n">
-        <v>4194877.7</v>
+        <v>4194863.8</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="14">
@@ -663,20 +667,20 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>54:35:061375:27</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D14" t="n">
-        <v>486345.35</v>
+        <v>486341.13</v>
       </c>
       <c r="E14" t="n">
-        <v>4194863.8</v>
+        <v>4194860.87</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="15">
@@ -685,20 +689,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>54:35:061375:27</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D15" t="n">
-        <v>486368.23</v>
+        <v>486331.18</v>
       </c>
       <c r="E15" t="n">
-        <v>4194879.66</v>
+        <v>4194852.88</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="16">
@@ -707,17 +711,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>54:35:061375:12</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D16" t="n">
-        <v>486241.67</v>
+        <v>486330.61</v>
       </c>
       <c r="E16" t="n">
-        <v>4194998.99</v>
+        <v>4194853.01</v>
       </c>
       <c r="F16" t="n">
         <v>0.3</v>
@@ -729,17 +733,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>54:35:061375:12</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D17" t="n">
-        <v>486237.45</v>
+        <v>486326.12</v>
       </c>
       <c r="E17" t="n">
-        <v>4194993.8</v>
+        <v>4194850.11</v>
       </c>
       <c r="F17" t="n">
         <v>0.3</v>
@@ -751,17 +755,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>54:35:061375:12</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D18" t="n">
-        <v>486233.37</v>
+        <v>486323.51</v>
       </c>
       <c r="E18" t="n">
-        <v>4194990.94</v>
+        <v>4194854.29</v>
       </c>
       <c r="F18" t="n">
         <v>0.3</v>
@@ -773,17 +777,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>54:35:061375:12</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D19" t="n">
-        <v>486211.77</v>
+        <v>486321.85</v>
       </c>
       <c r="E19" t="n">
-        <v>4194974.55</v>
+        <v>4194856.48</v>
       </c>
       <c r="F19" t="n">
         <v>0.3</v>
@@ -795,17 +799,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>54:35:061375:12</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D20" t="n">
-        <v>486211.47</v>
+        <v>486317.39</v>
       </c>
       <c r="E20" t="n">
-        <v>4194974.32</v>
+        <v>4194853.84</v>
       </c>
       <c r="F20" t="n">
         <v>0.3</v>
@@ -817,17 +821,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>54:35:061375:12</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D21" t="n">
-        <v>486213.98</v>
+        <v>486308.09</v>
       </c>
       <c r="E21" t="n">
-        <v>4194971.34</v>
+        <v>4194848.72</v>
       </c>
       <c r="F21" t="n">
         <v>0.3</v>
@@ -839,17 +843,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>54:35:061375:12</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D22" t="n">
-        <v>486220.93</v>
+        <v>486300.34</v>
       </c>
       <c r="E22" t="n">
-        <v>4194963</v>
+        <v>4194844.12</v>
       </c>
       <c r="F22" t="n">
         <v>0.3</v>
@@ -861,17 +865,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>54:35:061375:12</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D23" t="n">
-        <v>486224.46</v>
+        <v>486293.86</v>
       </c>
       <c r="E23" t="n">
-        <v>4194958.8</v>
+        <v>4194840.04</v>
       </c>
       <c r="F23" t="n">
         <v>0.3</v>
@@ -883,17 +887,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>54:35:061375:12</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D24" t="n">
-        <v>486257.08</v>
+        <v>486291.44</v>
       </c>
       <c r="E24" t="n">
-        <v>4194986.41</v>
+        <v>4194843.81</v>
       </c>
       <c r="F24" t="n">
         <v>0.3</v>
@@ -905,17 +909,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>54:35:061375:12</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D25" t="n">
-        <v>486241.67</v>
+        <v>486286.57</v>
       </c>
       <c r="E25" t="n">
-        <v>4194998.99</v>
+        <v>4194851.38</v>
       </c>
       <c r="F25" t="n">
         <v>0.3</v>
@@ -927,17 +931,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:11</t>
         </is>
       </c>
       <c r="C26" t="n">
         <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>486352.09</v>
+        <v>486280.32</v>
       </c>
       <c r="E26" t="n">
-        <v>4194844.99</v>
+        <v>4194861.75</v>
       </c>
       <c r="F26" t="n">
         <v>0.3</v>
@@ -949,17 +953,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D27" t="n">
-        <v>486375.65</v>
+        <v>486298.98</v>
       </c>
       <c r="E27" t="n">
-        <v>4194858.74</v>
+        <v>4194946.79</v>
       </c>
       <c r="F27" t="n">
         <v>0.3</v>
@@ -971,17 +975,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D28" t="n">
-        <v>486377.07</v>
+        <v>486295.93</v>
       </c>
       <c r="E28" t="n">
-        <v>4194857.05</v>
+        <v>4194948.91</v>
       </c>
       <c r="F28" t="n">
         <v>0.3</v>
@@ -993,17 +997,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D29" t="n">
-        <v>486380.44</v>
+        <v>486299.1</v>
       </c>
       <c r="E29" t="n">
-        <v>4194859.69</v>
+        <v>4194937.13</v>
       </c>
       <c r="F29" t="n">
         <v>0.3</v>
@@ -1015,17 +1019,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D30" t="n">
-        <v>486371.53</v>
+        <v>486301.25</v>
       </c>
       <c r="E30" t="n">
-        <v>4194869.99</v>
+        <v>4194938.38</v>
       </c>
       <c r="F30" t="n">
         <v>0.3</v>
@@ -1037,17 +1041,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D31" t="n">
-        <v>486372.68</v>
+        <v>486298.98</v>
       </c>
       <c r="E31" t="n">
-        <v>4194874.81</v>
+        <v>4194946.79</v>
       </c>
       <c r="F31" t="n">
         <v>0.3</v>
@@ -1059,17 +1063,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>486389.68</v>
+        <v>486314.19</v>
       </c>
       <c r="E32" t="n">
-        <v>4194857.13</v>
+        <v>4194934.85</v>
       </c>
       <c r="F32" t="n">
         <v>0.3</v>
@@ -1081,17 +1085,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D33" t="n">
-        <v>486397.19</v>
+        <v>486313.82</v>
       </c>
       <c r="E33" t="n">
-        <v>4194848.48</v>
+        <v>4194934.71</v>
       </c>
       <c r="F33" t="n">
         <v>0.3</v>
@@ -1103,17 +1107,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D34" t="n">
-        <v>486384.98</v>
+        <v>486307.81</v>
       </c>
       <c r="E34" t="n">
-        <v>4194840.22</v>
+        <v>4194929.27</v>
       </c>
       <c r="F34" t="n">
         <v>0.3</v>
@@ -1125,17 +1129,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D35" t="n">
-        <v>486380.36</v>
+        <v>486299.13</v>
       </c>
       <c r="E35" t="n">
-        <v>4194838.29</v>
+        <v>4194921.59</v>
       </c>
       <c r="F35" t="n">
         <v>0.3</v>
@@ -1147,17 +1151,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D36" t="n">
-        <v>486374.38</v>
+        <v>486296.74</v>
       </c>
       <c r="E36" t="n">
-        <v>4194835.23</v>
+        <v>4194919.3</v>
       </c>
       <c r="F36" t="n">
         <v>0.3</v>
@@ -1169,17 +1173,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D37" t="n">
-        <v>486357.77</v>
+        <v>486288.91</v>
       </c>
       <c r="E37" t="n">
-        <v>4194829.64</v>
+        <v>4194928.08</v>
       </c>
       <c r="F37" t="n">
         <v>0.3</v>
@@ -1191,17 +1195,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D38" t="n">
-        <v>486346.3</v>
+        <v>486292.44</v>
       </c>
       <c r="E38" t="n">
-        <v>4194828.05</v>
+        <v>4194930.83</v>
       </c>
       <c r="F38" t="n">
         <v>0.3</v>
@@ -1213,17 +1217,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D39" t="n">
-        <v>486340.47</v>
+        <v>486277.66</v>
       </c>
       <c r="E39" t="n">
-        <v>4194837.67</v>
+        <v>4194950</v>
       </c>
       <c r="F39" t="n">
         <v>0.3</v>
@@ -1235,17 +1239,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>54:35:061375:4</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D40" t="n">
-        <v>486352.09</v>
+        <v>486286.91</v>
       </c>
       <c r="E40" t="n">
-        <v>4194844.99</v>
+        <v>4194955.16</v>
       </c>
       <c r="F40" t="n">
         <v>0.3</v>
@@ -1257,20 +1261,20 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>54:35:061375:29</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D41" t="n">
-        <v>486295.86</v>
+        <v>486295.93</v>
       </c>
       <c r="E41" t="n">
-        <v>4194905.6</v>
+        <v>4194948.91</v>
       </c>
       <c r="F41" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="42">
@@ -1279,20 +1283,20 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>54:35:061375:29</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D42" t="n">
-        <v>486283.45</v>
+        <v>486298.98</v>
       </c>
       <c r="E42" t="n">
-        <v>4194921.92</v>
+        <v>4194946.79</v>
       </c>
       <c r="F42" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="43">
@@ -1301,20 +1305,20 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>54:35:061375:29</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D43" t="n">
-        <v>486282.59</v>
+        <v>486306.06</v>
       </c>
       <c r="E43" t="n">
-        <v>4194923.16</v>
+        <v>4194941.89</v>
       </c>
       <c r="F43" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="44">
@@ -1323,20 +1327,20 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>54:35:061375:29</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D44" t="n">
-        <v>486271.16</v>
+        <v>486311.37</v>
       </c>
       <c r="E44" t="n">
-        <v>4194914.29</v>
+        <v>4194938.08</v>
       </c>
       <c r="F44" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="45">
@@ -1345,20 +1349,20 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>54:35:061375:29</t>
+          <t>54:35:061375:9</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D45" t="n">
-        <v>486267.35</v>
+        <v>486314.19</v>
       </c>
       <c r="E45" t="n">
-        <v>4194911.46</v>
+        <v>4194934.85</v>
       </c>
       <c r="F45" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="46">
@@ -1367,20 +1371,20 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>54:35:061375:29</t>
+          <t>54:35:061375:12</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D46" t="n">
-        <v>486264.68</v>
+        <v>486241.67</v>
       </c>
       <c r="E46" t="n">
-        <v>4194909.52</v>
+        <v>4194998.99</v>
       </c>
       <c r="F46" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="47">
@@ -1389,20 +1393,20 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>54:35:061375:29</t>
+          <t>54:35:061375:12</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D47" t="n">
-        <v>486264.51</v>
+        <v>486237.45</v>
       </c>
       <c r="E47" t="n">
-        <v>4194908.88</v>
+        <v>4194993.8</v>
       </c>
       <c r="F47" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="48">
@@ -1411,20 +1415,20 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>54:35:061375:29</t>
+          <t>54:35:061375:12</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D48" t="n">
-        <v>486256.55</v>
+        <v>486233.37</v>
       </c>
       <c r="E48" t="n">
-        <v>4194903.8</v>
+        <v>4194990.94</v>
       </c>
       <c r="F48" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="49">
@@ -1433,20 +1437,20 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>54:35:061375:29</t>
+          <t>54:35:061375:12</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D49" t="n">
-        <v>486267.71</v>
+        <v>486211.77</v>
       </c>
       <c r="E49" t="n">
-        <v>4194885.93</v>
+        <v>4194974.55</v>
       </c>
       <c r="F49" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="50">
@@ -1455,20 +1459,20 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>54:35:061375:29</t>
+          <t>54:35:061375:12</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D50" t="n">
-        <v>486276.09</v>
+        <v>486211.47</v>
       </c>
       <c r="E50" t="n">
-        <v>4194891.62</v>
+        <v>4194974.32</v>
       </c>
       <c r="F50" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="51">
@@ -1477,20 +1481,20 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>54:35:061375:29</t>
+          <t>54:35:061375:12</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D51" t="n">
-        <v>486295.86</v>
+        <v>486213.98</v>
       </c>
       <c r="E51" t="n">
-        <v>4194905.6</v>
+        <v>4194971.34</v>
       </c>
       <c r="F51" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="52">
@@ -1499,17 +1503,17 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:12</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D52" t="n">
-        <v>486241.67</v>
+        <v>486220.93</v>
       </c>
       <c r="E52" t="n">
-        <v>4194998.99</v>
+        <v>4194963</v>
       </c>
       <c r="F52" t="n">
         <v>0.3</v>
@@ -1521,17 +1525,17 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:12</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D53" t="n">
-        <v>486237.45</v>
+        <v>486224.46</v>
       </c>
       <c r="E53" t="n">
-        <v>4194993.8</v>
+        <v>4194958.8</v>
       </c>
       <c r="F53" t="n">
         <v>0.3</v>
@@ -1543,17 +1547,17 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:12</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D54" t="n">
-        <v>486233.37</v>
+        <v>486257.08</v>
       </c>
       <c r="E54" t="n">
-        <v>4194990.94</v>
+        <v>4194986.41</v>
       </c>
       <c r="F54" t="n">
         <v>0.3</v>
@@ -1565,17 +1569,17 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:12</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D55" t="n">
-        <v>486211.77</v>
+        <v>486241.67</v>
       </c>
       <c r="E55" t="n">
-        <v>4194974.55</v>
+        <v>4194998.99</v>
       </c>
       <c r="F55" t="n">
         <v>0.3</v>
@@ -1587,17 +1591,17 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D56" t="n">
-        <v>486211.21</v>
+        <v>486302.97</v>
       </c>
       <c r="E56" t="n">
-        <v>4194974.12</v>
+        <v>4194910.64</v>
       </c>
       <c r="F56" t="n">
         <v>0.3</v>
@@ -1609,17 +1613,17 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D57" t="n">
-        <v>486203.77</v>
+        <v>486305.99</v>
       </c>
       <c r="E57" t="n">
-        <v>4194985.03</v>
+        <v>4194912.23</v>
       </c>
       <c r="F57" t="n">
         <v>0.3</v>
@@ -1631,17 +1635,17 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D58" t="n">
-        <v>486204.41</v>
+        <v>486311.83</v>
       </c>
       <c r="E58" t="n">
-        <v>4194985.31</v>
+        <v>4194916.68</v>
       </c>
       <c r="F58" t="n">
         <v>0.3</v>
@@ -1653,17 +1657,17 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D59" t="n">
-        <v>486203.14</v>
+        <v>486321.99</v>
       </c>
       <c r="E59" t="n">
-        <v>4194987.66</v>
+        <v>4194906.24</v>
       </c>
       <c r="F59" t="n">
         <v>0.3</v>
@@ -1675,17 +1679,17 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D60" t="n">
-        <v>486195.4</v>
+        <v>486298.48</v>
       </c>
       <c r="E60" t="n">
-        <v>4194999.31</v>
+        <v>4194888.08</v>
       </c>
       <c r="F60" t="n">
         <v>0.3</v>
@@ -1697,17 +1701,17 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D61" t="n">
-        <v>486215.25</v>
+        <v>486298.17</v>
       </c>
       <c r="E61" t="n">
-        <v>4195016.15</v>
+        <v>4194888.47</v>
       </c>
       <c r="F61" t="n">
         <v>0.3</v>
@@ -1719,17 +1723,17 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D62" t="n">
-        <v>486227.35</v>
+        <v>486289.1</v>
       </c>
       <c r="E62" t="n">
-        <v>4195005.26</v>
+        <v>4194881.36</v>
       </c>
       <c r="F62" t="n">
         <v>0.3</v>
@@ -1741,17 +1745,17 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D63" t="n">
-        <v>486231.14</v>
+        <v>486290.42</v>
       </c>
       <c r="E63" t="n">
-        <v>4195008.5</v>
+        <v>4194879.59</v>
       </c>
       <c r="F63" t="n">
         <v>0.3</v>
@@ -1763,17 +1767,17 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D64" t="n">
-        <v>486232</v>
+        <v>486276.66</v>
       </c>
       <c r="E64" t="n">
-        <v>4195007.17</v>
+        <v>4194870.04</v>
       </c>
       <c r="F64" t="n">
         <v>0.3</v>
@@ -1785,17 +1789,17 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D65" t="n">
-        <v>486233.43</v>
+        <v>486275.19</v>
       </c>
       <c r="E65" t="n">
-        <v>4195008.3</v>
+        <v>4194872.39</v>
       </c>
       <c r="F65" t="n">
         <v>0.3</v>
@@ -1807,17 +1811,17 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>54:35:061375:6</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D66" t="n">
-        <v>486241.67</v>
+        <v>486274.55</v>
       </c>
       <c r="E66" t="n">
-        <v>4194998.99</v>
+        <v>4194872.36</v>
       </c>
       <c r="F66" t="n">
         <v>0.3</v>
@@ -1829,20 +1833,20 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D67" t="n">
-        <v>486374.5</v>
+        <v>486269.22</v>
       </c>
       <c r="E67" t="n">
-        <v>4194865.81</v>
+        <v>4194882.19</v>
       </c>
       <c r="F67" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="68">
@@ -1851,20 +1855,20 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D68" t="n">
-        <v>486369.86</v>
+        <v>486269.48</v>
       </c>
       <c r="E68" t="n">
-        <v>4194871.06</v>
+        <v>4194882.36</v>
       </c>
       <c r="F68" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="69">
@@ -1873,20 +1877,20 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D69" t="n">
-        <v>486368.51</v>
+        <v>486267.5</v>
       </c>
       <c r="E69" t="n">
-        <v>4194869.87</v>
+        <v>4194885.49</v>
       </c>
       <c r="F69" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="70">
@@ -1895,20 +1899,20 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D70" t="n">
-        <v>486367.49</v>
+        <v>486267.84</v>
       </c>
       <c r="E70" t="n">
-        <v>4194871.02</v>
+        <v>4194885.72</v>
       </c>
       <c r="F70" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="71">
@@ -1917,20 +1921,20 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D71" t="n">
-        <v>486364.28</v>
+        <v>486267.71</v>
       </c>
       <c r="E71" t="n">
-        <v>4194868.16</v>
+        <v>4194885.93</v>
       </c>
       <c r="F71" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="72">
@@ -1939,20 +1943,20 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D72" t="n">
-        <v>486365.28</v>
+        <v>486276.09</v>
       </c>
       <c r="E72" t="n">
-        <v>4194867.01</v>
+        <v>4194891.62</v>
       </c>
       <c r="F72" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="73">
@@ -1961,20 +1965,20 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:5</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D73" t="n">
-        <v>486361.66</v>
+        <v>486302.97</v>
       </c>
       <c r="E73" t="n">
-        <v>4194863.79</v>
+        <v>4194910.64</v>
       </c>
       <c r="F73" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="74">
@@ -1983,20 +1987,20 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:3</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D74" t="n">
-        <v>486366.28</v>
+        <v>486277.66</v>
       </c>
       <c r="E74" t="n">
-        <v>4194858.55</v>
+        <v>4194950</v>
       </c>
       <c r="F74" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="75">
@@ -2005,20 +2009,20 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:3</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D75" t="n">
-        <v>486374.5</v>
+        <v>486292.44</v>
       </c>
       <c r="E75" t="n">
-        <v>4194865.81</v>
+        <v>4194930.83</v>
       </c>
       <c r="F75" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="76">
@@ -2027,17 +2031,17 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:3</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D76" t="n">
-        <v>486352.09</v>
+        <v>486288.91</v>
       </c>
       <c r="E76" t="n">
-        <v>4194844.99</v>
+        <v>4194928.08</v>
       </c>
       <c r="F76" t="n">
         <v>0.3</v>
@@ -2049,17 +2053,17 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:3</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D77" t="n">
-        <v>486375.65</v>
+        <v>486271.15</v>
       </c>
       <c r="E77" t="n">
-        <v>4194858.74</v>
+        <v>4194914.28</v>
       </c>
       <c r="F77" t="n">
         <v>0.3</v>
@@ -2071,17 +2075,17 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:3</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D78" t="n">
-        <v>486377.07</v>
+        <v>486267.35</v>
       </c>
       <c r="E78" t="n">
-        <v>4194857.05</v>
+        <v>4194911.46</v>
       </c>
       <c r="F78" t="n">
         <v>0.3</v>
@@ -2093,17 +2097,17 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:3</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D79" t="n">
-        <v>486380.44</v>
+        <v>486264.68</v>
       </c>
       <c r="E79" t="n">
-        <v>4194859.69</v>
+        <v>4194909.52</v>
       </c>
       <c r="F79" t="n">
         <v>0.3</v>
@@ -2115,17 +2119,17 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:3</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D80" t="n">
-        <v>486371.53</v>
+        <v>486249.14</v>
       </c>
       <c r="E80" t="n">
-        <v>4194869.99</v>
+        <v>4194934.52</v>
       </c>
       <c r="F80" t="n">
         <v>0.3</v>
@@ -2137,17 +2141,17 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:3</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D81" t="n">
-        <v>486372.68</v>
+        <v>486277.66</v>
       </c>
       <c r="E81" t="n">
-        <v>4194874.81</v>
+        <v>4194950</v>
       </c>
       <c r="F81" t="n">
         <v>0.3</v>
@@ -2159,11 +2163,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:27</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D82" t="n">
         <v>486368.23</v>
@@ -2172,7 +2176,7 @@
         <v>4194879.66</v>
       </c>
       <c r="F82" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="83">
@@ -2181,20 +2185,20 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:27</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D83" t="n">
-        <v>486341.13</v>
+        <v>486332.43</v>
       </c>
       <c r="E83" t="n">
-        <v>4194860.87</v>
+        <v>4194915.07</v>
       </c>
       <c r="F83" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="84">
@@ -2203,20 +2207,20 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>54:35:061375:1</t>
+          <t>54:35:061375:27</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D84" t="n">
-        <v>486352.09</v>
+        <v>486330.69</v>
       </c>
       <c r="E84" t="n">
-        <v>4194844.99</v>
+        <v>4194913.66</v>
       </c>
       <c r="F84" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="85">
@@ -2225,20 +2229,20 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:27</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D85" t="n">
-        <v>486298.98</v>
+        <v>486326.17</v>
       </c>
       <c r="E85" t="n">
-        <v>4194946.79</v>
+        <v>4194910.03</v>
       </c>
       <c r="F85" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="86">
@@ -2247,20 +2251,20 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:27</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D86" t="n">
-        <v>486295.93</v>
+        <v>486325.41</v>
       </c>
       <c r="E86" t="n">
-        <v>4194948.91</v>
+        <v>4194909.41</v>
       </c>
       <c r="F86" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="87">
@@ -2269,20 +2273,20 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:27</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D87" t="n">
-        <v>486299.1</v>
+        <v>486323.33</v>
       </c>
       <c r="E87" t="n">
-        <v>4194937.13</v>
+        <v>4194908.18</v>
       </c>
       <c r="F87" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="88">
@@ -2291,20 +2295,20 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:27</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D88" t="n">
-        <v>486301.25</v>
+        <v>486323.34</v>
       </c>
       <c r="E88" t="n">
-        <v>4194938.38</v>
+        <v>4194907.14</v>
       </c>
       <c r="F88" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="89">
@@ -2313,20 +2317,20 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:27</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D89" t="n">
-        <v>486298.98</v>
+        <v>486323.54</v>
       </c>
       <c r="E89" t="n">
-        <v>4194946.79</v>
+        <v>4194905.83</v>
       </c>
       <c r="F89" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="90">
@@ -2335,20 +2339,20 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:27</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D90" t="n">
-        <v>486314.19</v>
+        <v>486329.74</v>
       </c>
       <c r="E90" t="n">
-        <v>4194934.85</v>
+        <v>4194897.48</v>
       </c>
       <c r="F90" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="91">
@@ -2357,20 +2361,20 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:27</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D91" t="n">
-        <v>486313.82</v>
+        <v>486323.56</v>
       </c>
       <c r="E91" t="n">
-        <v>4194934.71</v>
+        <v>4194893.22</v>
       </c>
       <c r="F91" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="92">
@@ -2379,20 +2383,20 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:27</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D92" t="n">
-        <v>486307.81</v>
+        <v>486329.57</v>
       </c>
       <c r="E92" t="n">
-        <v>4194929.27</v>
+        <v>4194885.14</v>
       </c>
       <c r="F92" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="93">
@@ -2401,20 +2405,20 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:27</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D93" t="n">
-        <v>486299.13</v>
+        <v>486335.31</v>
       </c>
       <c r="E93" t="n">
-        <v>4194921.59</v>
+        <v>4194877.7</v>
       </c>
       <c r="F93" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="94">
@@ -2423,20 +2427,20 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:27</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D94" t="n">
-        <v>486296.74</v>
+        <v>486345.35</v>
       </c>
       <c r="E94" t="n">
-        <v>4194919.3</v>
+        <v>4194863.8</v>
       </c>
       <c r="F94" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="95">
@@ -2445,20 +2449,20 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:27</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D95" t="n">
-        <v>486288.91</v>
+        <v>486368.23</v>
       </c>
       <c r="E95" t="n">
-        <v>4194928.08</v>
+        <v>4194879.66</v>
       </c>
       <c r="F95" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="96">
@@ -2467,20 +2471,20 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:29</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D96" t="n">
-        <v>486292.44</v>
+        <v>486295.86</v>
       </c>
       <c r="E96" t="n">
-        <v>4194930.83</v>
+        <v>4194905.6</v>
       </c>
       <c r="F96" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="97">
@@ -2489,20 +2493,20 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:29</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D97" t="n">
-        <v>486277.66</v>
+        <v>486283.45</v>
       </c>
       <c r="E97" t="n">
-        <v>4194950</v>
+        <v>4194921.92</v>
       </c>
       <c r="F97" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="98">
@@ -2511,20 +2515,20 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:29</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D98" t="n">
-        <v>486286.91</v>
+        <v>486282.59</v>
       </c>
       <c r="E98" t="n">
-        <v>4194955.16</v>
+        <v>4194923.16</v>
       </c>
       <c r="F98" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="99">
@@ -2533,20 +2537,20 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:29</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D99" t="n">
-        <v>486295.93</v>
+        <v>486271.16</v>
       </c>
       <c r="E99" t="n">
-        <v>4194948.91</v>
+        <v>4194914.29</v>
       </c>
       <c r="F99" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="100">
@@ -2555,20 +2559,20 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:29</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D100" t="n">
-        <v>486298.98</v>
+        <v>486267.35</v>
       </c>
       <c r="E100" t="n">
-        <v>4194946.79</v>
+        <v>4194911.46</v>
       </c>
       <c r="F100" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="101">
@@ -2577,20 +2581,20 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:29</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D101" t="n">
-        <v>486306.06</v>
+        <v>486264.68</v>
       </c>
       <c r="E101" t="n">
-        <v>4194941.89</v>
+        <v>4194909.52</v>
       </c>
       <c r="F101" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="102">
@@ -2599,20 +2603,20 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:29</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D102" t="n">
-        <v>486311.37</v>
+        <v>486264.51</v>
       </c>
       <c r="E102" t="n">
-        <v>4194938.08</v>
+        <v>4194908.88</v>
       </c>
       <c r="F102" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="103">
@@ -2621,20 +2625,20 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>54:35:061375:9</t>
+          <t>54:35:061375:29</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D103" t="n">
-        <v>486314.19</v>
+        <v>486256.55</v>
       </c>
       <c r="E103" t="n">
-        <v>4194934.85</v>
+        <v>4194903.8</v>
       </c>
       <c r="F103" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="104">
@@ -2643,20 +2647,20 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>54:35:061375:8</t>
+          <t>54:35:061375:29</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D104" t="n">
-        <v>486326.17</v>
+        <v>486267.71</v>
       </c>
       <c r="E104" t="n">
-        <v>4194910.03</v>
+        <v>4194885.93</v>
       </c>
       <c r="F104" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="105">
@@ -2665,20 +2669,20 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>54:35:061375:8</t>
+          <t>54:35:061375:29</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D105" t="n">
-        <v>486330.69</v>
+        <v>486276.09</v>
       </c>
       <c r="E105" t="n">
-        <v>4194913.66</v>
+        <v>4194891.62</v>
       </c>
       <c r="F105" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="106">
@@ -2687,20 +2691,20 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>54:35:061375:8</t>
+          <t>54:35:061375:29</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="D106" t="n">
-        <v>486326.09</v>
+        <v>486295.86</v>
       </c>
       <c r="E106" t="n">
-        <v>4194913.25</v>
+        <v>4194905.6</v>
       </c>
       <c r="F106" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="107">
@@ -2713,13 +2717,13 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D107" t="n">
-        <v>486324.58</v>
+        <v>486326.17</v>
       </c>
       <c r="E107" t="n">
-        <v>4194911.95</v>
+        <v>4194910.03</v>
       </c>
       <c r="F107" t="n">
         <v>0.3</v>
@@ -2735,13 +2739,13 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D108" t="n">
-        <v>486326.17</v>
+        <v>486330.69</v>
       </c>
       <c r="E108" t="n">
-        <v>4194910.03</v>
+        <v>4194913.66</v>
       </c>
       <c r="F108" t="n">
         <v>0.3</v>
@@ -2757,13 +2761,13 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D109" t="n">
-        <v>486326.17</v>
+        <v>486326.09</v>
       </c>
       <c r="E109" t="n">
-        <v>4194910.03</v>
+        <v>4194913.25</v>
       </c>
       <c r="F109" t="n">
         <v>0.3</v>
@@ -2779,13 +2783,13 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D110" t="n">
-        <v>486330.69</v>
+        <v>486324.58</v>
       </c>
       <c r="E110" t="n">
-        <v>4194913.66</v>
+        <v>4194911.95</v>
       </c>
       <c r="F110" t="n">
         <v>0.3</v>
@@ -2801,13 +2805,13 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D111" t="n">
-        <v>486332.43</v>
+        <v>486326.17</v>
       </c>
       <c r="E111" t="n">
-        <v>4194915.07</v>
+        <v>4194910.03</v>
       </c>
       <c r="F111" t="n">
         <v>0.3</v>
@@ -2823,13 +2827,13 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D112" t="n">
-        <v>486314.19</v>
+        <v>486326.17</v>
       </c>
       <c r="E112" t="n">
-        <v>4194934.85</v>
+        <v>4194910.03</v>
       </c>
       <c r="F112" t="n">
         <v>0.3</v>
@@ -2845,13 +2849,13 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D113" t="n">
-        <v>486313.82</v>
+        <v>486330.69</v>
       </c>
       <c r="E113" t="n">
-        <v>4194934.71</v>
+        <v>4194913.66</v>
       </c>
       <c r="F113" t="n">
         <v>0.3</v>
@@ -2867,13 +2871,13 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D114" t="n">
-        <v>486307.81</v>
+        <v>486332.43</v>
       </c>
       <c r="E114" t="n">
-        <v>4194929.27</v>
+        <v>4194915.07</v>
       </c>
       <c r="F114" t="n">
         <v>0.3</v>
@@ -2889,13 +2893,13 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D115" t="n">
-        <v>486299.13</v>
+        <v>486314.19</v>
       </c>
       <c r="E115" t="n">
-        <v>4194921.59</v>
+        <v>4194934.85</v>
       </c>
       <c r="F115" t="n">
         <v>0.3</v>
@@ -2911,13 +2915,13 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D116" t="n">
-        <v>486296.74</v>
+        <v>486313.82</v>
       </c>
       <c r="E116" t="n">
-        <v>4194919.3</v>
+        <v>4194934.71</v>
       </c>
       <c r="F116" t="n">
         <v>0.3</v>
@@ -2933,13 +2937,13 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D117" t="n">
-        <v>486302.97</v>
+        <v>486307.81</v>
       </c>
       <c r="E117" t="n">
-        <v>4194910.64</v>
+        <v>4194929.27</v>
       </c>
       <c r="F117" t="n">
         <v>0.3</v>
@@ -2955,13 +2959,13 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D118" t="n">
-        <v>486305.99</v>
+        <v>486299.13</v>
       </c>
       <c r="E118" t="n">
-        <v>4194912.23</v>
+        <v>4194921.59</v>
       </c>
       <c r="F118" t="n">
         <v>0.3</v>
@@ -2977,13 +2981,13 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D119" t="n">
-        <v>486311.83</v>
+        <v>486296.74</v>
       </c>
       <c r="E119" t="n">
-        <v>4194916.68</v>
+        <v>4194919.3</v>
       </c>
       <c r="F119" t="n">
         <v>0.3</v>
@@ -2999,13 +3003,13 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D120" t="n">
-        <v>486321.99</v>
+        <v>486302.97</v>
       </c>
       <c r="E120" t="n">
-        <v>4194906.24</v>
+        <v>4194910.64</v>
       </c>
       <c r="F120" t="n">
         <v>0.3</v>
@@ -3021,13 +3025,13 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D121" t="n">
-        <v>486298.48</v>
+        <v>486305.99</v>
       </c>
       <c r="E121" t="n">
-        <v>4194888.08</v>
+        <v>4194912.23</v>
       </c>
       <c r="F121" t="n">
         <v>0.3</v>
@@ -3043,13 +3047,13 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D122" t="n">
-        <v>486298.17</v>
+        <v>486311.83</v>
       </c>
       <c r="E122" t="n">
-        <v>4194888.47</v>
+        <v>4194916.68</v>
       </c>
       <c r="F122" t="n">
         <v>0.3</v>
@@ -3065,13 +3069,13 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D123" t="n">
-        <v>486289.1</v>
+        <v>486321.99</v>
       </c>
       <c r="E123" t="n">
-        <v>4194881.36</v>
+        <v>4194906.24</v>
       </c>
       <c r="F123" t="n">
         <v>0.3</v>
@@ -3087,13 +3091,13 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D124" t="n">
-        <v>486290.42</v>
+        <v>486298.48</v>
       </c>
       <c r="E124" t="n">
-        <v>4194879.59</v>
+        <v>4194888.08</v>
       </c>
       <c r="F124" t="n">
         <v>0.3</v>
@@ -3109,13 +3113,13 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D125" t="n">
-        <v>486276.66</v>
+        <v>486298.17</v>
       </c>
       <c r="E125" t="n">
-        <v>4194870.04</v>
+        <v>4194888.47</v>
       </c>
       <c r="F125" t="n">
         <v>0.3</v>
@@ -3131,13 +3135,13 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D126" t="n">
-        <v>486276.05</v>
+        <v>486289.1</v>
       </c>
       <c r="E126" t="n">
-        <v>4194869.52</v>
+        <v>4194881.36</v>
       </c>
       <c r="F126" t="n">
         <v>0.3</v>
@@ -3153,13 +3157,13 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D127" t="n">
-        <v>486280.32</v>
+        <v>486290.42</v>
       </c>
       <c r="E127" t="n">
-        <v>4194861.75</v>
+        <v>4194879.59</v>
       </c>
       <c r="F127" t="n">
         <v>0.3</v>
@@ -3175,13 +3179,13 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D128" t="n">
-        <v>486287.28</v>
+        <v>486276.66</v>
       </c>
       <c r="E128" t="n">
-        <v>4194866.48</v>
+        <v>4194870.04</v>
       </c>
       <c r="F128" t="n">
         <v>0.3</v>
@@ -3197,13 +3201,13 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D129" t="n">
-        <v>486299.2</v>
+        <v>486276.05</v>
       </c>
       <c r="E129" t="n">
-        <v>4194875.36</v>
+        <v>4194869.52</v>
       </c>
       <c r="F129" t="n">
         <v>0.3</v>
@@ -3219,13 +3223,13 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D130" t="n">
-        <v>486323.27</v>
+        <v>486280.32</v>
       </c>
       <c r="E130" t="n">
-        <v>4194893.02</v>
+        <v>4194861.75</v>
       </c>
       <c r="F130" t="n">
         <v>0.3</v>
@@ -3241,16 +3245,16 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D131" t="n">
-        <v>486323.56</v>
+        <v>486287.28</v>
       </c>
       <c r="E131" t="n">
-        <v>4194893.22</v>
+        <v>4194866.48</v>
       </c>
       <c r="F131" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="132">
@@ -3263,13 +3267,13 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D132" t="n">
-        <v>486329.74</v>
+        <v>486299.2</v>
       </c>
       <c r="E132" t="n">
-        <v>4194897.48</v>
+        <v>4194875.36</v>
       </c>
       <c r="F132" t="n">
         <v>0.3</v>
@@ -3285,13 +3289,13 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D133" t="n">
-        <v>486323.54</v>
+        <v>486323.27</v>
       </c>
       <c r="E133" t="n">
-        <v>4194905.83</v>
+        <v>4194893.02</v>
       </c>
       <c r="F133" t="n">
         <v>0.3</v>
@@ -3307,16 +3311,16 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D134" t="n">
-        <v>486323.34</v>
+        <v>486323.56</v>
       </c>
       <c r="E134" t="n">
-        <v>4194907.14</v>
+        <v>4194893.22</v>
       </c>
       <c r="F134" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="135">
@@ -3329,13 +3333,13 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D135" t="n">
-        <v>486323.33</v>
+        <v>486329.74</v>
       </c>
       <c r="E135" t="n">
-        <v>4194908.18</v>
+        <v>4194897.48</v>
       </c>
       <c r="F135" t="n">
         <v>0.3</v>
@@ -3351,13 +3355,13 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D136" t="n">
-        <v>486325.41</v>
+        <v>486323.54</v>
       </c>
       <c r="E136" t="n">
-        <v>4194909.41</v>
+        <v>4194905.83</v>
       </c>
       <c r="F136" t="n">
         <v>0.3</v>
@@ -3373,13 +3377,13 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D137" t="n">
-        <v>486326.17</v>
+        <v>486323.34</v>
       </c>
       <c r="E137" t="n">
-        <v>4194910.03</v>
+        <v>4194907.14</v>
       </c>
       <c r="F137" t="n">
         <v>0.3</v>
@@ -3391,17 +3395,17 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:8</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D138" t="n">
-        <v>486293.86</v>
+        <v>486323.33</v>
       </c>
       <c r="E138" t="n">
-        <v>4194840.04</v>
+        <v>4194908.18</v>
       </c>
       <c r="F138" t="n">
         <v>0.3</v>
@@ -3413,22 +3417,20 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:8</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D139" t="n">
-        <v>486293.58</v>
+        <v>486325.41</v>
       </c>
       <c r="E139" t="n">
-        <v>4194840.47</v>
-      </c>
-      <c r="F139" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+        <v>4194909.41</v>
+      </c>
+      <c r="F139" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="140">
@@ -3437,22 +3439,20 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:8</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="D140" t="n">
-        <v>486294.71</v>
+        <v>486326.17</v>
       </c>
       <c r="E140" t="n">
-        <v>4194840.58</v>
-      </c>
-      <c r="F140" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+        <v>4194910.03</v>
+      </c>
+      <c r="F140" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="141">
@@ -3461,17 +3461,17 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D141" t="n">
-        <v>486293.86</v>
+        <v>486241.67</v>
       </c>
       <c r="E141" t="n">
-        <v>4194840.04</v>
+        <v>4194998.99</v>
       </c>
       <c r="F141" t="n">
         <v>0.3</v>
@@ -3483,17 +3483,17 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D142" t="n">
-        <v>486280.32</v>
+        <v>486237.45</v>
       </c>
       <c r="E142" t="n">
-        <v>4194861.75</v>
+        <v>4194993.8</v>
       </c>
       <c r="F142" t="n">
         <v>0.3</v>
@@ -3505,17 +3505,17 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D143" t="n">
-        <v>486287.28</v>
+        <v>486233.37</v>
       </c>
       <c r="E143" t="n">
-        <v>4194866.48</v>
+        <v>4194990.94</v>
       </c>
       <c r="F143" t="n">
         <v>0.3</v>
@@ -3527,17 +3527,17 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D144" t="n">
-        <v>486299.2</v>
+        <v>486211.77</v>
       </c>
       <c r="E144" t="n">
-        <v>4194875.36</v>
+        <v>4194974.55</v>
       </c>
       <c r="F144" t="n">
         <v>0.3</v>
@@ -3549,17 +3549,17 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D145" t="n">
-        <v>486323.27</v>
+        <v>486211.21</v>
       </c>
       <c r="E145" t="n">
-        <v>4194893.02</v>
+        <v>4194974.12</v>
       </c>
       <c r="F145" t="n">
         <v>0.3</v>
@@ -3571,17 +3571,17 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D146" t="n">
-        <v>486323.56</v>
+        <v>486203.77</v>
       </c>
       <c r="E146" t="n">
-        <v>4194893.22</v>
+        <v>4194985.03</v>
       </c>
       <c r="F146" t="n">
         <v>0.3</v>
@@ -3593,17 +3593,17 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D147" t="n">
-        <v>486329.57</v>
+        <v>486204.41</v>
       </c>
       <c r="E147" t="n">
-        <v>4194885.14</v>
+        <v>4194985.31</v>
       </c>
       <c r="F147" t="n">
         <v>0.3</v>
@@ -3615,17 +3615,17 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D148" t="n">
-        <v>486335.31</v>
+        <v>486203.14</v>
       </c>
       <c r="E148" t="n">
-        <v>4194877.7</v>
+        <v>4194987.66</v>
       </c>
       <c r="F148" t="n">
         <v>0.3</v>
@@ -3637,17 +3637,17 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D149" t="n">
-        <v>486345.35</v>
+        <v>486195.4</v>
       </c>
       <c r="E149" t="n">
-        <v>4194863.8</v>
+        <v>4194999.31</v>
       </c>
       <c r="F149" t="n">
         <v>0.3</v>
@@ -3659,17 +3659,17 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D150" t="n">
-        <v>486341.13</v>
+        <v>486215.25</v>
       </c>
       <c r="E150" t="n">
-        <v>4194860.87</v>
+        <v>4195016.15</v>
       </c>
       <c r="F150" t="n">
         <v>0.3</v>
@@ -3681,17 +3681,17 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D151" t="n">
-        <v>486331.18</v>
+        <v>486227.35</v>
       </c>
       <c r="E151" t="n">
-        <v>4194852.88</v>
+        <v>4195005.26</v>
       </c>
       <c r="F151" t="n">
         <v>0.3</v>
@@ -3703,17 +3703,17 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D152" t="n">
-        <v>486330.61</v>
+        <v>486231.14</v>
       </c>
       <c r="E152" t="n">
-        <v>4194853.01</v>
+        <v>4195008.5</v>
       </c>
       <c r="F152" t="n">
         <v>0.3</v>
@@ -3725,17 +3725,17 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D153" t="n">
-        <v>486326.12</v>
+        <v>486232</v>
       </c>
       <c r="E153" t="n">
-        <v>4194850.11</v>
+        <v>4195007.17</v>
       </c>
       <c r="F153" t="n">
         <v>0.3</v>
@@ -3747,17 +3747,17 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D154" t="n">
-        <v>486323.51</v>
+        <v>486233.43</v>
       </c>
       <c r="E154" t="n">
-        <v>4194854.29</v>
+        <v>4195008.3</v>
       </c>
       <c r="F154" t="n">
         <v>0.3</v>
@@ -3769,17 +3769,17 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:6</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D155" t="n">
-        <v>486321.85</v>
+        <v>486241.67</v>
       </c>
       <c r="E155" t="n">
-        <v>4194856.48</v>
+        <v>4194998.99</v>
       </c>
       <c r="F155" t="n">
         <v>0.3</v>
@@ -3791,20 +3791,20 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D156" t="n">
-        <v>486317.39</v>
+        <v>486374.5</v>
       </c>
       <c r="E156" t="n">
-        <v>4194853.84</v>
+        <v>4194865.81</v>
       </c>
       <c r="F156" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="157">
@@ -3813,20 +3813,20 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D157" t="n">
-        <v>486308.09</v>
+        <v>486369.86</v>
       </c>
       <c r="E157" t="n">
-        <v>4194848.72</v>
+        <v>4194871.06</v>
       </c>
       <c r="F157" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="158">
@@ -3835,20 +3835,20 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D158" t="n">
-        <v>486300.34</v>
+        <v>486368.51</v>
       </c>
       <c r="E158" t="n">
-        <v>4194844.12</v>
+        <v>4194869.87</v>
       </c>
       <c r="F158" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="159">
@@ -3857,20 +3857,20 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D159" t="n">
-        <v>486293.86</v>
+        <v>486367.49</v>
       </c>
       <c r="E159" t="n">
-        <v>4194840.04</v>
+        <v>4194871.02</v>
       </c>
       <c r="F159" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="160">
@@ -3879,20 +3879,20 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D160" t="n">
-        <v>486291.44</v>
+        <v>486364.28</v>
       </c>
       <c r="E160" t="n">
-        <v>4194843.81</v>
+        <v>4194868.16</v>
       </c>
       <c r="F160" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="161">
@@ -3901,20 +3901,20 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D161" t="n">
-        <v>486286.57</v>
+        <v>486365.28</v>
       </c>
       <c r="E161" t="n">
-        <v>4194851.38</v>
+        <v>4194867.01</v>
       </c>
       <c r="F161" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="162">
@@ -3923,20 +3923,20 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>54:35:061375:11</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D162" t="n">
-        <v>486280.32</v>
+        <v>486361.66</v>
       </c>
       <c r="E162" t="n">
-        <v>4194861.75</v>
+        <v>4194863.79</v>
       </c>
       <c r="F162" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="163">
@@ -3945,20 +3945,20 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>54:35:061375:3</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D163" t="n">
-        <v>486277.66</v>
+        <v>486366.28</v>
       </c>
       <c r="E163" t="n">
-        <v>4194950</v>
+        <v>4194858.55</v>
       </c>
       <c r="F163" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="164">
@@ -3967,20 +3967,20 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>54:35:061375:3</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D164" t="n">
-        <v>486292.44</v>
+        <v>486374.5</v>
       </c>
       <c r="E164" t="n">
-        <v>4194930.83</v>
+        <v>4194865.81</v>
       </c>
       <c r="F164" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="165">
@@ -3989,17 +3989,17 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>54:35:061375:3</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D165" t="n">
-        <v>486288.91</v>
+        <v>486352.09</v>
       </c>
       <c r="E165" t="n">
-        <v>4194928.08</v>
+        <v>4194844.99</v>
       </c>
       <c r="F165" t="n">
         <v>0.3</v>
@@ -4011,17 +4011,17 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>54:35:061375:3</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D166" t="n">
-        <v>486271.15</v>
+        <v>486375.65</v>
       </c>
       <c r="E166" t="n">
-        <v>4194914.28</v>
+        <v>4194858.74</v>
       </c>
       <c r="F166" t="n">
         <v>0.3</v>
@@ -4033,17 +4033,17 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>54:35:061375:3</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D167" t="n">
-        <v>486267.35</v>
+        <v>486377.07</v>
       </c>
       <c r="E167" t="n">
-        <v>4194911.46</v>
+        <v>4194857.05</v>
       </c>
       <c r="F167" t="n">
         <v>0.3</v>
@@ -4055,17 +4055,17 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>54:35:061375:3</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D168" t="n">
-        <v>486264.68</v>
+        <v>486380.44</v>
       </c>
       <c r="E168" t="n">
-        <v>4194909.52</v>
+        <v>4194859.69</v>
       </c>
       <c r="F168" t="n">
         <v>0.3</v>
@@ -4077,17 +4077,17 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>54:35:061375:3</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D169" t="n">
-        <v>486249.14</v>
+        <v>486371.53</v>
       </c>
       <c r="E169" t="n">
-        <v>4194934.52</v>
+        <v>4194869.99</v>
       </c>
       <c r="F169" t="n">
         <v>0.3</v>
@@ -4099,17 +4099,17 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>54:35:061375:3</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D170" t="n">
-        <v>486277.66</v>
+        <v>486372.68</v>
       </c>
       <c r="E170" t="n">
-        <v>4194950</v>
+        <v>4194874.81</v>
       </c>
       <c r="F170" t="n">
         <v>0.3</v>
@@ -4121,17 +4121,17 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D171" t="n">
-        <v>486302.97</v>
+        <v>486368.23</v>
       </c>
       <c r="E171" t="n">
-        <v>4194910.64</v>
+        <v>4194879.66</v>
       </c>
       <c r="F171" t="n">
         <v>0.3</v>
@@ -4143,17 +4143,17 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D172" t="n">
-        <v>486305.99</v>
+        <v>486341.13</v>
       </c>
       <c r="E172" t="n">
-        <v>4194912.23</v>
+        <v>4194860.87</v>
       </c>
       <c r="F172" t="n">
         <v>0.3</v>
@@ -4165,17 +4165,17 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:1</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D173" t="n">
-        <v>486311.83</v>
+        <v>486352.09</v>
       </c>
       <c r="E173" t="n">
-        <v>4194916.68</v>
+        <v>4194844.99</v>
       </c>
       <c r="F173" t="n">
         <v>0.3</v>
@@ -4187,17 +4187,17 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D174" t="n">
-        <v>486321.99</v>
+        <v>486352.09</v>
       </c>
       <c r="E174" t="n">
-        <v>4194906.24</v>
+        <v>4194844.99</v>
       </c>
       <c r="F174" t="n">
         <v>0.3</v>
@@ -4209,17 +4209,17 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D175" t="n">
-        <v>486298.48</v>
+        <v>486375.65</v>
       </c>
       <c r="E175" t="n">
-        <v>4194888.08</v>
+        <v>4194858.74</v>
       </c>
       <c r="F175" t="n">
         <v>0.3</v>
@@ -4231,17 +4231,17 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D176" t="n">
-        <v>486298.17</v>
+        <v>486377.07</v>
       </c>
       <c r="E176" t="n">
-        <v>4194888.47</v>
+        <v>4194857.05</v>
       </c>
       <c r="F176" t="n">
         <v>0.3</v>
@@ -4253,17 +4253,17 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D177" t="n">
-        <v>486289.1</v>
+        <v>486380.44</v>
       </c>
       <c r="E177" t="n">
-        <v>4194881.36</v>
+        <v>4194859.69</v>
       </c>
       <c r="F177" t="n">
         <v>0.3</v>
@@ -4275,17 +4275,17 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D178" t="n">
-        <v>486290.42</v>
+        <v>486371.53</v>
       </c>
       <c r="E178" t="n">
-        <v>4194879.59</v>
+        <v>4194869.99</v>
       </c>
       <c r="F178" t="n">
         <v>0.3</v>
@@ -4297,17 +4297,17 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D179" t="n">
-        <v>486276.66</v>
+        <v>486372.68</v>
       </c>
       <c r="E179" t="n">
-        <v>4194870.04</v>
+        <v>4194874.81</v>
       </c>
       <c r="F179" t="n">
         <v>0.3</v>
@@ -4319,17 +4319,17 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D180" t="n">
-        <v>486275.19</v>
+        <v>486389.68</v>
       </c>
       <c r="E180" t="n">
-        <v>4194872.39</v>
+        <v>4194857.13</v>
       </c>
       <c r="F180" t="n">
         <v>0.3</v>
@@ -4341,17 +4341,17 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D181" t="n">
-        <v>486274.55</v>
+        <v>486397.19</v>
       </c>
       <c r="E181" t="n">
-        <v>4194872.36</v>
+        <v>4194848.48</v>
       </c>
       <c r="F181" t="n">
         <v>0.3</v>
@@ -4363,17 +4363,17 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D182" t="n">
-        <v>486269.22</v>
+        <v>486384.98</v>
       </c>
       <c r="E182" t="n">
-        <v>4194882.19</v>
+        <v>4194840.22</v>
       </c>
       <c r="F182" t="n">
         <v>0.3</v>
@@ -4385,17 +4385,17 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D183" t="n">
-        <v>486269.48</v>
+        <v>486380.36</v>
       </c>
       <c r="E183" t="n">
-        <v>4194882.36</v>
+        <v>4194838.29</v>
       </c>
       <c r="F183" t="n">
         <v>0.3</v>
@@ -4407,17 +4407,17 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D184" t="n">
-        <v>486267.5</v>
+        <v>486374.38</v>
       </c>
       <c r="E184" t="n">
-        <v>4194885.49</v>
+        <v>4194835.23</v>
       </c>
       <c r="F184" t="n">
         <v>0.3</v>
@@ -4429,17 +4429,17 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D185" t="n">
-        <v>486267.84</v>
+        <v>486357.77</v>
       </c>
       <c r="E185" t="n">
-        <v>4194885.72</v>
+        <v>4194829.64</v>
       </c>
       <c r="F185" t="n">
         <v>0.3</v>
@@ -4451,17 +4451,17 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D186" t="n">
-        <v>486267.71</v>
+        <v>486346.3</v>
       </c>
       <c r="E186" t="n">
-        <v>4194885.93</v>
+        <v>4194828.05</v>
       </c>
       <c r="F186" t="n">
         <v>0.3</v>
@@ -4473,17 +4473,17 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D187" t="n">
-        <v>486276.09</v>
+        <v>486340.47</v>
       </c>
       <c r="E187" t="n">
-        <v>4194891.62</v>
+        <v>4194837.67</v>
       </c>
       <c r="F187" t="n">
         <v>0.3</v>
@@ -4495,17 +4495,17 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>54:35:061375:5</t>
+          <t>54:35:061375:4</t>
         </is>
       </c>
       <c r="C188" t="n">
         <v>1</v>
       </c>
       <c r="D188" t="n">
-        <v>486302.97</v>
+        <v>486352.09</v>
       </c>
       <c r="E188" t="n">
-        <v>4194910.64</v>
+        <v>4194844.99</v>
       </c>
       <c r="F188" t="n">
         <v>0.3</v>

</xml_diff>